<commit_message>
More EPPlus coverage closes #37
</commit_message>
<xml_diff>
--- a/OLT.Libraries.UnitTest/Assets/Resources/ImportTest.xlsx
+++ b/OLT.Libraries.UnitTest/Assets/Resources/ImportTest.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\GitHub\olt-dotnet-libraries\OLT.Libraries.UnitTest\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C91B7-14B1-45F0-A423-F9EABBA15C67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75B60DD-173E-4963-B5BA-23364C66AA7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{93978094-454C-4CFE-9B3E-F331438EFBB7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{93978094-454C-4CFE-9B3E-F331438EFBB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="50">
   <si>
     <t>Grade</t>
   </si>
@@ -169,6 +170,21 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Literals</t>
+  </si>
+  <si>
+    <t>"Test"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  100  </t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -222,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,6 +256,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8E6D82-E1D5-4627-9BA0-5E14B411819A}">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -566,7 +583,7 @@
     <col min="2" max="8" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -591,8 +608,14 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -617,8 +640,12 @@
       <c r="H2" s="5">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="e">
+        <f>SUM(H2 I3)</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -644,7 +671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -667,10 +694,10 @@
         <v>8</v>
       </c>
       <c r="H4" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -696,10 +723,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>29</v>
-      </c>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -718,11 +743,15 @@
       <c r="G6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="5">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6">
+        <f>IF(ISBLANK(A6), 10, 1000)</f>
+        <v>10</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -747,8 +776,11 @@
       <c r="H7" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -773,8 +805,11 @@
       <c r="H8" s="5">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -800,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -826,7 +861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -852,7 +887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -862,7 +897,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:10">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -872,7 +907,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -882,7 +917,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -892,7 +927,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1525,4 +1560,333 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D263FBA-6608-4135-A948-06B13287E41A}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="29">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5">
+        <v>37</v>
+      </c>
+      <c r="I2" t="e">
+        <f>SUM(H2 I3)</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6">
+        <f>IF(ISBLANK(A6), 10, 1000)</f>
+        <v>10</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="5">
+        <v>19</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="5">
+        <v>67</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>